<commit_message>
Quick Select using the mid and front pivot
</commit_message>
<xml_diff>
--- a/Data Structure/Graph/Graph.xlsx
+++ b/Data Structure/Graph/Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamrathod/Documents/Study Material/DS/DataStructure-And-Algorithm/Data Structure/Graph/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2770347-2DDE-3246-B92B-2CFE04ABA90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997166AF-6D0D-F144-B738-A3B1B0D71460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4E42177B-4881-CA45-8674-08098C02AC7A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Number</t>
   </si>
@@ -45,8 +45,12 @@
     <t>Explanation</t>
   </si>
   <si>
+    <t>Graph</t>
+  </si>
+  <si>
     <t>1. Come Up with a Brute Force Approach
 4. Always check for base case.
+Adjacency Matrix:
 Difference:
     preReq = { i:[] for i in range(numCourses)}
         print(preReq)
@@ -58,14 +62,17 @@
         {1: []}</t>
   </si>
   <si>
-    <t>Graph</t>
+    <t>210. Course Schedule II</t>
+  </si>
+  <si>
+    <t>207. Course Schedule I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -97,6 +104,20 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF212121"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -131,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -153,6 +174,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -469,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4A21D9-BFC5-D744-9210-5766C92121CA}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,7 +511,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -501,7 +528,7 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" ht="390" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -521,8 +548,200 @@
       <c r="A6" s="2">
         <v>1</v>
       </c>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" s="3"/>
     </row>
+    <row r="7" spans="1:3" s="9" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="17" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="18" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="19" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="20" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="21" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="22" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="23" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="24" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="25" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="26" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="27" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="28" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="29" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="30" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="31" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="32" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="33" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="34" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="35" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="36" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="37" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="38" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="39" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="40" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="41" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="42" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="43" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="44" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="45" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="46" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="47" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="48" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="49" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="50" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="51" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="52" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="53" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="54" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="55" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="56" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="57" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="58" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="59" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="60" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="61" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="62" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="63" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="64" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="65" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="66" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="67" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="68" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="69" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="70" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="71" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="72" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="73" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="74" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="75" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="76" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="77" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="78" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="79" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="80" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="81" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="82" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="83" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="84" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="85" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="86" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="87" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="88" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="89" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="90" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="91" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="92" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="93" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="94" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="95" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="96" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="97" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="98" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="99" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="100" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="101" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="102" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="103" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="104" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="105" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="106" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="107" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="108" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="109" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="110" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="111" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="112" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="113" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="114" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="115" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="116" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="117" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="118" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="119" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="120" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="121" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="122" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="123" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="124" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="125" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="126" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="127" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="128" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="129" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="130" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="131" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="132" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="133" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="134" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="135" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="136" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="137" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="138" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="139" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="140" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="141" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="142" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="143" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="144" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="145" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="146" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="147" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="148" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="149" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="150" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="151" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="152" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="153" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="154" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="155" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="156" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="157" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="158" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="159" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="160" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="161" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="162" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="163" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="164" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="165" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="166" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="167" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="168" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="169" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="170" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="171" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="172" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="173" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="174" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="175" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="176" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="177" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="178" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="179" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="180" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="181" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="182" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="183" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="184" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="185" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="186" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="187" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
+    <row r="188" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C3"/>

</xml_diff>